<commit_message>
Sequential and Simultaneous Games in LINGO
</commit_message>
<xml_diff>
--- a/results/utility_comparison.xlsx
+++ b/results/utility_comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ayush\Documents\GitHub\budgeted-attack-defense-game\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF08FCAF-6E10-42B6-BDDC-1EB8F7CC7695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB688A7E-89A0-4F07-BAF3-FCF38DA52D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{AE22A0F3-9994-42E2-9DA4-6155FB65E00A}"/>
+    <workbookView xWindow="600" yWindow="564" windowWidth="17280" windowHeight="9420" xr2:uid="{AE22A0F3-9994-42E2-9DA4-6155FB65E00A}"/>
   </bookViews>
   <sheets>
     <sheet name="Simultaneous Game" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>T1</t>
   </si>
@@ -114,10 +114,19 @@
     <t>B (Attacker's valuations)</t>
   </si>
   <si>
-    <t>Random 100 Sample</t>
-  </si>
-  <si>
-    <t>LHS 100 Sample</t>
+    <t>LHS 100 + Algorithm 1 [It30]</t>
+  </si>
+  <si>
+    <t>Random 100 Sample (Simultaneous)</t>
+  </si>
+  <si>
+    <t>LHS 100 Sample  (Simultaneous)</t>
+  </si>
+  <si>
+    <t>(Sequential)</t>
+  </si>
+  <si>
+    <t>(Simultaneous)</t>
   </si>
 </sst>
 </file>
@@ -178,12 +187,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,15 +509,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{906086F2-6FD1-40B3-A591-ECC6A24454BE}">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" zoomScale="77" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="21.21875" customWidth="1"/>
+    <col min="1" max="1" width="34.21875" customWidth="1"/>
+    <col min="2" max="2" width="21.21875" customWidth="1"/>
     <col min="3" max="3" width="9.109375" customWidth="1"/>
     <col min="13" max="13" width="14.5546875" customWidth="1"/>
     <col min="14" max="14" width="13.5546875" customWidth="1"/>
@@ -552,93 +563,99 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="5">
+        <v>1.0940000000000001</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="E2" s="5">
+        <v>2.91</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="H2" s="5">
+        <v>1.71</v>
+      </c>
+      <c r="I2" s="5">
+        <v>22.425999999999998</v>
+      </c>
+      <c r="J2" s="5">
+        <v>2.6379999999999999</v>
+      </c>
+      <c r="K2" s="5">
+        <v>0</v>
+      </c>
+      <c r="L2" s="5">
+        <v>3.226</v>
+      </c>
+      <c r="M2" s="5">
+        <v>92.215000000000003</v>
+      </c>
+      <c r="N2" s="5">
+        <v>38.08</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
         <v>0.61399999999999999</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>1.349</v>
       </c>
-      <c r="E2">
+      <c r="E3">
         <v>2.6850000000000001</v>
       </c>
-      <c r="F2">
+      <c r="F3">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="G2">
+      <c r="G3">
         <v>0.34499999999999997</v>
       </c>
-      <c r="H2">
+      <c r="H3">
         <v>2.99</v>
       </c>
-      <c r="I2">
+      <c r="I3">
         <v>19.303000000000001</v>
       </c>
-      <c r="J2">
+      <c r="J3">
         <v>3.762</v>
       </c>
-      <c r="K2">
+      <c r="K3">
         <v>0.32800000000000001</v>
       </c>
-      <c r="L2">
+      <c r="L3">
         <v>3.6179999999999999</v>
       </c>
-      <c r="M2">
+      <c r="M3">
         <v>111.22799999999999</v>
       </c>
-      <c r="N2">
+      <c r="N3">
         <v>32.055999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.74347516458795604</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1.7881015162034899</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1.7629148814139499</v>
-      </c>
-      <c r="F3" s="2">
-        <v>3.70802993191175E-10</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0.70550843742379099</v>
-      </c>
-      <c r="H3" s="3">
-        <v>7.7174661504955999</v>
-      </c>
-      <c r="I3" s="3">
-        <v>11.840730141162901</v>
-      </c>
-      <c r="J3" s="3">
-        <v>2.5500718766633301E-10</v>
-      </c>
-      <c r="K3" s="3">
-        <v>2.2509224833959798</v>
-      </c>
-      <c r="L3" s="3">
-        <v>8.1908812246904308</v>
-      </c>
-      <c r="M3" s="3">
-        <v>203.236476118799</v>
-      </c>
-      <c r="N3" s="3">
-        <v>34.2674878868321</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="C4" s="2">
         <v>0.74347516458795604</v>
@@ -671,59 +688,59 @@
         <v>8.1908812246904308</v>
       </c>
       <c r="M4" s="3">
+        <v>203.236476118799</v>
+      </c>
+      <c r="N4" s="3">
+        <v>34.2674878868321</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.74347516458795604</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.7881015162034899</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.7629148814139499</v>
+      </c>
+      <c r="F5" s="2">
+        <v>3.70802993191175E-10</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.70550843742379099</v>
+      </c>
+      <c r="H5" s="3">
+        <v>7.7174661504955999</v>
+      </c>
+      <c r="I5" s="3">
+        <v>11.840730141162901</v>
+      </c>
+      <c r="J5" s="3">
+        <v>2.5500718766633301E-10</v>
+      </c>
+      <c r="K5" s="3">
+        <v>2.2509224833959798</v>
+      </c>
+      <c r="L5" s="3">
+        <v>8.1908812246904308</v>
+      </c>
+      <c r="M5" s="3">
         <v>195.40263835925401</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N5" s="3">
         <v>63.645786280100602</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0.63848277537828002</v>
-      </c>
-      <c r="D5" s="3">
-        <v>1.9083583402025699</v>
-      </c>
-      <c r="E5" s="3">
-        <v>1.7320472192359</v>
-      </c>
-      <c r="F5" s="3">
-        <v>5.1262199652025997E-10</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0.72111166467062204</v>
-      </c>
-      <c r="H5" s="3">
-        <v>4.1480431136359899</v>
-      </c>
-      <c r="I5" s="3">
-        <v>12.308270050940401</v>
-      </c>
-      <c r="J5" s="3">
-        <v>1.4099032282805699E-11</v>
-      </c>
-      <c r="K5" s="3">
-        <v>5.4463450099867501</v>
-      </c>
-      <c r="L5" s="3">
-        <v>8.0973418254226797</v>
-      </c>
-      <c r="M5" s="3">
-        <v>193.351738483639</v>
-      </c>
-      <c r="N5" s="3">
-        <v>33.649110621024697</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="C6" s="3">
         <v>0.63848277537828002</v>
@@ -756,109 +773,194 @@
         <v>8.0973418254226797</v>
       </c>
       <c r="M6" s="3">
+        <v>193.351738483639</v>
+      </c>
+      <c r="N6" s="3">
+        <v>33.649110621024697</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.63848277537828002</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.9083583402025699</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1.7320472192359</v>
+      </c>
+      <c r="F7" s="3">
+        <v>5.1262199652025997E-10</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.72111166467062204</v>
+      </c>
+      <c r="H7" s="3">
+        <v>4.1480431136359899</v>
+      </c>
+      <c r="I7" s="3">
+        <v>12.308270050940401</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1.4099032282805699E-11</v>
+      </c>
+      <c r="K7" s="3">
+        <v>5.4463450099867501</v>
+      </c>
+      <c r="L7" s="3">
+        <v>8.0973418254226797</v>
+      </c>
+      <c r="M7" s="3">
         <v>201.84219755917999</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N7" s="3">
         <v>64.830836602408297</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="1"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="3">
+        <v>9.9961735335147794E-2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2.8920905517928399</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2.00794771287201</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3">
+        <v>3.3636669470585798</v>
+      </c>
+      <c r="I8" s="3">
+        <v>11.7418724411864</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.86284213594438497</v>
+      </c>
+      <c r="K8" s="3">
+        <v>5.60606672269234</v>
+      </c>
+      <c r="L8" s="3">
+        <v>8.4255517531182704</v>
+      </c>
+      <c r="M8" s="3">
+        <v>232.04573444936099</v>
+      </c>
+      <c r="N8" s="3">
+        <v>53.984592023317703</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="1"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>25</v>
       </c>
-      <c r="B16">
+      <c r="B18">
         <v>20</v>
       </c>
-      <c r="C16">
+      <c r="C18">
         <v>100</v>
       </c>
-      <c r="D16">
+      <c r="D18">
         <v>50</v>
       </c>
-      <c r="E16">
+      <c r="E18">
         <v>2</v>
       </c>
-      <c r="F16">
+      <c r="F18">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>24</v>
       </c>
-      <c r="B17">
+      <c r="B19">
         <v>70</v>
       </c>
-      <c r="C17">
+      <c r="C19">
         <v>1000</v>
       </c>
-      <c r="D17">
+      <c r="D19">
         <v>50</v>
       </c>
-      <c r="E17">
+      <c r="E19">
         <v>75</v>
       </c>
-      <c r="F17">
+      <c r="F19">
         <v>150</v>
       </c>
     </row>

</xml_diff>